<commit_message>
Update data package at: 2025-09-26T20:18:39Z
</commit_message>
<xml_diff>
--- a/data-raw/memoria_calculo.xlsx
+++ b/data-raw/memoria_calculo.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuário\Desktop\00 planejamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cecad365.sharepoint.com/sites/Splor/Documentos Compartilhados/General/@dcppn/DCPPN 2026/PPAG e LOA 2026/material de apoio/material de apoio - gerar volumes/2026/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{665C75EF-4BBF-4902-8AF5-2F86FDB50838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1796EFC-945B-4206-AAD2-FEBE2DAA1810}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{665C75EF-4BBF-4902-8AF5-2F86FDB50838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DB429F0-1246-48FF-AAA1-C76BBE3BC3F9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="segurança alimentar" sheetId="1" r:id="rId1"/>
+    <sheet name="criança e adolescente" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'criança e adolescente'!$A$1:$D$75</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'segurança alimentar'!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="104">
   <si>
     <t>ACAO_COD</t>
   </si>
@@ -201,13 +203,163 @@
   </si>
   <si>
     <t>UNIVERSALIZAÇÃO DOS SERVIÇOS DE SANEAMENTO NA ÁREA DE ATUAÇÃO DA COPANOR</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>Lazer</t>
+  </si>
+  <si>
+    <t>Desporto Comunitário</t>
+  </si>
+  <si>
+    <t>Saneamento Básico Urbano</t>
+  </si>
+  <si>
+    <t>Saneamento Básico Rural</t>
+  </si>
+  <si>
+    <t>Serviços Urbanos</t>
+  </si>
+  <si>
+    <t>Infra-Estrutura Urbana</t>
+  </si>
+  <si>
+    <t>Habitação Urbana</t>
+  </si>
+  <si>
+    <t>Habitação Rural</t>
+  </si>
+  <si>
+    <t>Outros Encargos Especiais</t>
+  </si>
+  <si>
+    <t>Outras Transferências</t>
+  </si>
+  <si>
+    <t>Assistência aos Povos Indígenas</t>
+  </si>
+  <si>
+    <t>Direitos Individuais, Coletivos e Difusos</t>
+  </si>
+  <si>
+    <t>Custódia e Reintegração Social</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Assistência à Criança e ao Adolescente</t>
+  </si>
+  <si>
+    <t>Difusão Cultural</t>
+  </si>
+  <si>
+    <t>Transferências para a Educação Básica</t>
+  </si>
+  <si>
+    <t>Transportes Especiais</t>
+  </si>
+  <si>
+    <t>Difusão do Conhecimento Científico e Tecnológico</t>
+  </si>
+  <si>
+    <t>Desenvolvimento Tecnológico e Engenharia</t>
+  </si>
+  <si>
+    <t>Desenvolvimento Científico</t>
+  </si>
+  <si>
+    <t>Educação Básica</t>
+  </si>
+  <si>
+    <t>Educação Especial</t>
+  </si>
+  <si>
+    <t>Educação de Jovens e Adultos</t>
+  </si>
+  <si>
+    <t>Educação Infantil</t>
+  </si>
+  <si>
+    <t>Ensino Profissional</t>
+  </si>
+  <si>
+    <t>Ensino Médio</t>
+  </si>
+  <si>
+    <t>Ensino Fundamental</t>
+  </si>
+  <si>
+    <t>Alimentação e Nutrição</t>
+  </si>
+  <si>
+    <t>Comunicação Social</t>
+  </si>
+  <si>
+    <t>Formação de Recursos Humanos</t>
+  </si>
+  <si>
+    <t>Tecnologia da Informação</t>
+  </si>
+  <si>
+    <t>Controle Interno</t>
+  </si>
+  <si>
+    <t>Administração Financeira</t>
+  </si>
+  <si>
+    <t>Administração Geral</t>
+  </si>
+  <si>
+    <t>Planejamento e Orçamento</t>
+  </si>
+  <si>
+    <t>Vigilância Epidemiológica</t>
+  </si>
+  <si>
+    <t>Vigilância Sanitária</t>
+  </si>
+  <si>
+    <t>Suporte Profilático e Terapêutico</t>
+  </si>
+  <si>
+    <t>Assistência Hospitalar e Ambulatorial</t>
+  </si>
+  <si>
+    <t>Atenção Básica</t>
+  </si>
+  <si>
+    <t>Fomento ao Trabalho</t>
+  </si>
+  <si>
+    <t>Empregabilidade</t>
+  </si>
+  <si>
+    <t>Assistência Comunitária</t>
+  </si>
+  <si>
+    <t>Assistência ao Portador de Deficiência</t>
+  </si>
+  <si>
+    <t>NE/E</t>
+  </si>
+  <si>
+    <t>SUBFUNCAO_DESC</t>
+  </si>
+  <si>
+    <t>SUBFUNCAO_COD</t>
+  </si>
+  <si>
+    <t>FUNCAO_COD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +392,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -277,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -292,6 +450,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,17 +739,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A36" workbookViewId="0">
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -592,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1025</v>
       </c>
@@ -600,7 +765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1026</v>
       </c>
@@ -608,7 +773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1028</v>
       </c>
@@ -616,7 +781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1034</v>
       </c>
@@ -624,7 +789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1053</v>
       </c>
@@ -632,7 +797,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1082</v>
       </c>
@@ -640,7 +805,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1089</v>
       </c>
@@ -648,7 +813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>2033</v>
       </c>
@@ -656,7 +821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>2101</v>
       </c>
@@ -664,7 +829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>2102</v>
       </c>
@@ -672,7 +837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2116</v>
       </c>
@@ -680,7 +845,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>4016</v>
       </c>
@@ -688,7 +853,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>4018</v>
       </c>
@@ -696,7 +861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>4019</v>
       </c>
@@ -704,7 +869,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>4023</v>
       </c>
@@ -712,7 +877,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>4037</v>
       </c>
@@ -720,7 +885,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>4044</v>
       </c>
@@ -728,7 +893,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>4056</v>
       </c>
@@ -736,7 +901,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>4126</v>
       </c>
@@ -744,7 +909,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>4147</v>
       </c>
@@ -752,7 +917,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>4151</v>
       </c>
@@ -760,7 +925,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>4154</v>
       </c>
@@ -768,7 +933,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>4157</v>
       </c>
@@ -776,7 +941,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>4196</v>
       </c>
@@ -784,7 +949,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>4197</v>
       </c>
@@ -792,7 +957,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>4202</v>
       </c>
@@ -800,7 +965,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>4203</v>
       </c>
@@ -808,7 +973,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>4206</v>
       </c>
@@ -816,7 +981,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>4235</v>
       </c>
@@ -824,7 +989,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>4236</v>
       </c>
@@ -832,7 +997,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>4238</v>
       </c>
@@ -840,7 +1005,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>4320</v>
       </c>
@@ -848,7 +1013,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>4323</v>
       </c>
@@ -856,7 +1021,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>4325</v>
       </c>
@@ -864,7 +1029,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>4358</v>
       </c>
@@ -872,7 +1037,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>4359</v>
       </c>
@@ -880,7 +1045,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>4361</v>
       </c>
@@ -888,7 +1053,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>4363</v>
       </c>
@@ -896,7 +1061,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>4398</v>
       </c>
@@ -904,7 +1069,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>4399</v>
       </c>
@@ -912,7 +1077,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>4400</v>
       </c>
@@ -920,7 +1085,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>4405</v>
       </c>
@@ -928,7 +1093,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>4412</v>
       </c>
@@ -936,7 +1101,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>4416</v>
       </c>
@@ -944,7 +1109,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>4419</v>
       </c>
@@ -952,7 +1117,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>4420</v>
       </c>
@@ -960,7 +1125,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>4474</v>
       </c>
@@ -968,7 +1133,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>4510</v>
       </c>
@@ -976,7 +1141,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>4516</v>
       </c>
@@ -984,7 +1149,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>4544</v>
       </c>
@@ -992,7 +1157,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>8008</v>
       </c>
@@ -1000,7 +1165,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>8012</v>
       </c>
@@ -1018,7 +1183,1104 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA42A560-EC7E-4F51-9582-6A1F57862B12}">
+  <dimension ref="A1:D75"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="54.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>8</v>
+      </c>
+      <c r="B2" s="9">
+        <v>121</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>8</v>
+      </c>
+      <c r="B3" s="9">
+        <v>122</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9">
+        <v>123</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>8</v>
+      </c>
+      <c r="B5" s="9">
+        <v>124</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>8</v>
+      </c>
+      <c r="B6" s="9">
+        <v>126</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>8</v>
+      </c>
+      <c r="B7" s="9">
+        <v>128</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>8</v>
+      </c>
+      <c r="B8" s="9">
+        <v>131</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9">
+        <v>242</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9">
+        <v>243</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9">
+        <v>244</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>8</v>
+      </c>
+      <c r="B12" s="9">
+        <v>333</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>8</v>
+      </c>
+      <c r="B13" s="9">
+        <v>334</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="9">
+        <v>363</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>8</v>
+      </c>
+      <c r="B15" s="9">
+        <v>423</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>8</v>
+      </c>
+      <c r="B16" s="9">
+        <v>571</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>8</v>
+      </c>
+      <c r="B17" s="9">
+        <v>572</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>8</v>
+      </c>
+      <c r="B18" s="9">
+        <v>573</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>8</v>
+      </c>
+      <c r="B19" s="9">
+        <v>845</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>10</v>
+      </c>
+      <c r="B20" s="9">
+        <v>121</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>10</v>
+      </c>
+      <c r="B21" s="9">
+        <v>122</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>10</v>
+      </c>
+      <c r="B22" s="9">
+        <v>123</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>10</v>
+      </c>
+      <c r="B23" s="9">
+        <v>124</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>10</v>
+      </c>
+      <c r="B24" s="9">
+        <v>126</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>10</v>
+      </c>
+      <c r="B25" s="9">
+        <v>128</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>10</v>
+      </c>
+      <c r="B26" s="9">
+        <v>131</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>10</v>
+      </c>
+      <c r="B27" s="9">
+        <v>301</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>10</v>
+      </c>
+      <c r="B28" s="9">
+        <v>302</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>10</v>
+      </c>
+      <c r="B29" s="9">
+        <v>303</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>10</v>
+      </c>
+      <c r="B30" s="9">
+        <v>304</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
+        <v>10</v>
+      </c>
+      <c r="B31" s="9">
+        <v>305</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
+        <v>10</v>
+      </c>
+      <c r="B32" s="9">
+        <v>306</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>10</v>
+      </c>
+      <c r="B33" s="9">
+        <v>571</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>10</v>
+      </c>
+      <c r="B34" s="9">
+        <v>572</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
+        <v>10</v>
+      </c>
+      <c r="B35" s="9">
+        <v>573</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
+        <v>12</v>
+      </c>
+      <c r="B36" s="9">
+        <v>121</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
+        <v>12</v>
+      </c>
+      <c r="B37" s="9">
+        <v>122</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
+        <v>12</v>
+      </c>
+      <c r="B38" s="9">
+        <v>123</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
+        <v>12</v>
+      </c>
+      <c r="B39" s="9">
+        <v>124</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>12</v>
+      </c>
+      <c r="B40" s="9">
+        <v>126</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
+        <v>12</v>
+      </c>
+      <c r="B41" s="9">
+        <v>128</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
+        <v>12</v>
+      </c>
+      <c r="B42" s="9">
+        <v>131</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
+        <v>12</v>
+      </c>
+      <c r="B43" s="9">
+        <v>243</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="9">
+        <v>12</v>
+      </c>
+      <c r="B44" s="9">
+        <v>306</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="9">
+        <v>12</v>
+      </c>
+      <c r="B45" s="9">
+        <v>361</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="9">
+        <v>12</v>
+      </c>
+      <c r="B46" s="9">
+        <v>362</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="9">
+        <v>12</v>
+      </c>
+      <c r="B47" s="9">
+        <v>363</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="9">
+        <v>12</v>
+      </c>
+      <c r="B48" s="9">
+        <v>365</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="9">
+        <v>12</v>
+      </c>
+      <c r="B49" s="9">
+        <v>366</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="9">
+        <v>12</v>
+      </c>
+      <c r="B50" s="9">
+        <v>367</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="9">
+        <v>12</v>
+      </c>
+      <c r="B51" s="9">
+        <v>368</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="9">
+        <v>12</v>
+      </c>
+      <c r="B52" s="9">
+        <v>423</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="9">
+        <v>12</v>
+      </c>
+      <c r="B53" s="9">
+        <v>571</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="9">
+        <v>12</v>
+      </c>
+      <c r="B54" s="9">
+        <v>572</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="9">
+        <v>12</v>
+      </c>
+      <c r="B55" s="9">
+        <v>573</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="9">
+        <v>12</v>
+      </c>
+      <c r="B56" s="9">
+        <v>785</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="9">
+        <v>12</v>
+      </c>
+      <c r="B57" s="9">
+        <v>845</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="9">
+        <v>12</v>
+      </c>
+      <c r="B58" s="9">
+        <v>847</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="9">
+        <v>13</v>
+      </c>
+      <c r="B59" s="9">
+        <v>392</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="9">
+        <v>14</v>
+      </c>
+      <c r="B60" s="9">
+        <v>243</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="9">
+        <v>14</v>
+      </c>
+      <c r="B61" s="9">
+        <v>421</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="9">
+        <v>14</v>
+      </c>
+      <c r="B62" s="9">
+        <v>422</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="9">
+        <v>14</v>
+      </c>
+      <c r="B63" s="9">
+        <v>423</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="9">
+        <v>14</v>
+      </c>
+      <c r="B64" s="9">
+        <v>813</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="9">
+        <v>14</v>
+      </c>
+      <c r="B65" s="9">
+        <v>845</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="9">
+        <v>14</v>
+      </c>
+      <c r="B66" s="9">
+        <v>846</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="9">
+        <v>16</v>
+      </c>
+      <c r="B67" s="9">
+        <v>451</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="9">
+        <v>16</v>
+      </c>
+      <c r="B68" s="9">
+        <v>481</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="9">
+        <v>16</v>
+      </c>
+      <c r="B69" s="9">
+        <v>482</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="9">
+        <v>17</v>
+      </c>
+      <c r="B70" s="9">
+        <v>451</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="9">
+        <v>17</v>
+      </c>
+      <c r="B71" s="9">
+        <v>452</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="9">
+        <v>17</v>
+      </c>
+      <c r="B72" s="9">
+        <v>511</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="9">
+        <v>17</v>
+      </c>
+      <c r="B73" s="9">
+        <v>512</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="9">
+        <v>27</v>
+      </c>
+      <c r="B74" s="9">
+        <v>812</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="9">
+        <v>27</v>
+      </c>
+      <c r="B75" s="9">
+        <v>813</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="19" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="7797dc5feb179b4da55a9ebddd321181">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="90078f443198b6d5c0fd169535a443b9" ns2:_="" ns3:_="">
     <xsd:import namespace="6f4338ef-addb-4c87-aefe-1895241b335f"/>
@@ -1279,41 +2541,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3A4A5B7-B008-4619-B816-1F4ADC3379B1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1911C249-B410-40D2-907C-22C001E41BF2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D93B3A83-D183-4C54-A570-09F5A1AE63ED}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D93B3A83-D183-4C54-A570-09F5A1AE63ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b91e7f20-fe0a-487d-91a9-605ac1c64acf"/>
+    <ds:schemaRef ds:uri="6f4338ef-addb-4c87-aefe-1895241b335f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1911C249-B410-40D2-907C-22C001E41BF2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3A4A5B7-B008-4619-B816-1F4ADC3379B1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6f4338ef-addb-4c87-aefe-1895241b335f"/>
+    <ds:schemaRef ds:uri="b91e7f20-fe0a-487d-91a9-605ac1c64acf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>